<commit_message>
Project Report for sprint 2
</commit_message>
<xml_diff>
--- a/Team7ProjectReport.xlsx
+++ b/Team7ProjectReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/Week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA468895-FDEC-2948-821E-8C50D0212DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F705A11-5EBF-244C-A2F8-D0F9A0FF59AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="500" windowWidth="23260" windowHeight="13180" activeTab="5" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="198">
   <si>
     <t>First</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -534,9 +534,6 @@
     <t>Children should be born after marriage of parents (and not more than 9 months after their divorce)</t>
   </si>
   <si>
-    <t>Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
     <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
   </si>
   <si>
@@ -637,6 +634,18 @@
   </si>
   <si>
     <t>completed</t>
+  </si>
+  <si>
+    <t>getting each team member equally involved in the task. Taking everyone's feedback by doing informal peer-reviews.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irrelevant discussions during the meetings. </t>
+  </si>
+  <si>
+    <t>Communication gaps</t>
+  </si>
+  <si>
+    <t>Child should be born before the death of the mother and before 9 months after the death of the father</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1259,7 @@
                   <c:v>45106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45117</c:v>
+                  <c:v>45120</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>45133</c:v>
@@ -1268,10 +1277,16 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3487,7 +3502,7 @@
   <dimension ref="A3:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3561,19 +3576,19 @@
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -3629,7 +3644,7 @@
   <dimension ref="A3:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3666,10 +3681,10 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3683,10 +3698,10 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3703,7 +3718,7 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3720,7 +3735,7 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3737,7 +3752,7 @@
         <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3754,7 +3769,7 @@
         <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3771,7 +3786,7 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3788,7 +3803,7 @@
         <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3802,10 +3817,10 @@
         <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3819,10 +3834,10 @@
         <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3839,7 +3854,7 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3856,7 +3871,7 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3873,7 +3888,7 @@
         <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3890,7 +3905,7 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3907,7 +3922,7 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3924,7 +3939,7 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3937,6 +3952,12 @@
       <c r="C20" t="s">
         <v>74</v>
       </c>
+      <c r="D20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -3948,6 +3969,12 @@
       <c r="C21" t="s">
         <v>75</v>
       </c>
+      <c r="D21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -3959,6 +3986,12 @@
       <c r="C22" t="s">
         <v>76</v>
       </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -3970,6 +4003,12 @@
       <c r="C23" t="s">
         <v>77</v>
       </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -3981,6 +4020,12 @@
       <c r="C24" t="s">
         <v>78</v>
       </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -3992,6 +4037,12 @@
       <c r="C25" t="s">
         <v>79</v>
       </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -4003,6 +4054,12 @@
       <c r="C26" t="s">
         <v>80</v>
       </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -4013,6 +4070,12 @@
       </c>
       <c r="C27" t="s">
         <v>81</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4113,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2ECB25-720D-8D47-86EC-308937FE2D00}">
   <dimension ref="A3:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4227,11 +4290,14 @@
       <c r="C21" s="12">
         <v>24</v>
       </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
       <c r="E21" s="11">
         <v>330</v>
       </c>
       <c r="F21" s="11">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -4245,11 +4311,14 @@
       <c r="C22" s="12">
         <v>16</v>
       </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
       <c r="E22" s="11">
-        <v>0</v>
+        <v>589</v>
       </c>
       <c r="F22" s="11">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="G22" s="7"/>
     </row>
@@ -4263,6 +4332,9 @@
       <c r="C23" s="12">
         <v>8</v>
       </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
       <c r="E23" s="11">
         <v>0</v>
       </c>
@@ -4280,6 +4352,9 @@
       </c>
       <c r="C24" s="12">
         <v>0</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
       </c>
       <c r="E24" s="11">
         <v>0</v>
@@ -4304,7 +4379,7 @@
   <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4349,7 +4424,7 @@
         <v>45092</v>
       </c>
       <c r="B4" s="21">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -4357,8 +4432,8 @@
       <c r="D4">
         <v>330</v>
       </c>
-      <c r="E4">
-        <v>210</v>
+      <c r="E4" s="11">
+        <v>165</v>
       </c>
       <c r="F4">
         <v>160</v>
@@ -4369,17 +4444,35 @@
         <v>45106</v>
       </c>
       <c r="B5" s="12">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>589</v>
+      </c>
+      <c r="E5" s="11">
+        <v>145</v>
+      </c>
+      <c r="F5">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
-        <v>45117</v>
+        <v>45120</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>45133</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -4393,12 +4486,12 @@
   <dimension ref="A2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39" style="27" customWidth="1"/>
   </cols>
@@ -4440,10 +4533,10 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
         <v>188</v>
-      </c>
-      <c r="D3" t="s">
-        <v>189</v>
       </c>
       <c r="E3" s="5">
         <v>5</v>
@@ -4467,10 +4560,10 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
         <v>188</v>
-      </c>
-      <c r="D4" t="s">
-        <v>189</v>
       </c>
       <c r="E4" s="5">
         <v>5</v>
@@ -4497,7 +4590,7 @@
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="5">
         <v>5</v>
@@ -4524,7 +4617,7 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E6" s="5">
         <v>5</v>
@@ -4551,7 +4644,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E7" s="5">
         <v>5</v>
@@ -4578,7 +4671,7 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E8" s="5">
         <v>5</v>
@@ -4605,7 +4698,7 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E9" s="5">
         <v>5</v>
@@ -4626,13 +4719,13 @@
         <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E10" s="17">
         <v>5</v>
@@ -4650,18 +4743,18 @@
     </row>
     <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="K14" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="L14" s="27" t="s">
         <v>190</v>
-      </c>
-      <c r="L14" s="27" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="17" spans="11:12" ht="34" x14ac:dyDescent="0.2">
       <c r="K17" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="L17" s="27" t="s">
         <v>192</v>
-      </c>
-      <c r="L17" s="27" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4672,19 +4765,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5BDE68-3A09-9D41-98E9-14B644F01EC8}">
-  <dimension ref="A3:I11"/>
+  <dimension ref="A3:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.83203125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>108</v>
       </c>
@@ -4713,26 +4807,37 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
         <v>188</v>
       </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E4" s="17">
+        <v>35</v>
+      </c>
+      <c r="F4" s="5">
+        <v>40</v>
+      </c>
+      <c r="G4" s="17">
+        <v>40</v>
+      </c>
+      <c r="H4" s="5">
+        <v>20</v>
+      </c>
+      <c r="I4" s="18">
+        <v>45120</v>
+      </c>
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -4740,18 +4845,29 @@
         <v>67</v>
       </c>
       <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
         <v>188</v>
       </c>
-      <c r="D5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E5" s="17">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="17">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>25</v>
+      </c>
+      <c r="I5" s="18">
+        <v>45120</v>
+      </c>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -4762,15 +4878,26 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="E6" s="17">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5">
+        <v>30</v>
+      </c>
+      <c r="G6" s="17">
+        <v>38</v>
+      </c>
+      <c r="H6" s="17">
+        <v>15</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45118</v>
+      </c>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -4781,15 +4908,26 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="E7" s="17">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5">
+        <v>30</v>
+      </c>
+      <c r="G7" s="17">
+        <v>45</v>
+      </c>
+      <c r="H7" s="17">
+        <v>20</v>
+      </c>
+      <c r="I7" s="18">
+        <v>45118</v>
+      </c>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -4800,15 +4938,26 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="E8" s="17">
+        <v>15</v>
+      </c>
+      <c r="F8" s="5">
+        <v>30</v>
+      </c>
+      <c r="G8" s="17">
+        <v>29</v>
+      </c>
+      <c r="H8" s="17">
+        <v>15</v>
+      </c>
+      <c r="I8" s="18">
+        <v>45119</v>
+      </c>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -4819,15 +4968,26 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="E9" s="17">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5">
+        <v>40</v>
+      </c>
+      <c r="G9" s="17">
+        <v>17</v>
+      </c>
+      <c r="H9" s="17">
+        <v>20</v>
+      </c>
+      <c r="I9" s="18">
+        <v>45119</v>
+      </c>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -4838,15 +4998,25 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="E10" s="17">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5">
+        <v>40</v>
+      </c>
+      <c r="G10" s="17">
+        <v>20</v>
+      </c>
+      <c r="H10" s="17">
+        <v>15</v>
+      </c>
+      <c r="I10" s="18">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -4857,13 +5027,44 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
+        <v>188</v>
+      </c>
+      <c r="E11" s="17">
+        <v>20</v>
+      </c>
+      <c r="F11" s="17">
+        <v>30</v>
+      </c>
+      <c r="G11" s="17">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17">
+        <v>15</v>
+      </c>
+      <c r="I11" s="18">
+        <v>45118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="K12" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="K14" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L15" s="27" t="s">
+        <v>196</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4872,12 +5073,160 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4605CCB-00E7-694D-83D4-7E84E084E5F6}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4900,8 +5249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E792817E-5E9F-5543-BCFF-41F35057F086}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4998,26 +5347,26 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -5028,7 +5377,7 @@
         <v>67</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5039,7 +5388,7 @@
         <v>68</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -5050,7 +5399,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -5061,7 +5410,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5072,7 +5421,7 @@
         <v>71</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5083,7 +5432,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5094,7 +5443,7 @@
         <v>73</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5105,7 +5454,7 @@
         <v>74</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5116,7 +5465,7 @@
         <v>75</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5127,7 +5476,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5138,7 +5487,7 @@
         <v>77</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5149,7 +5498,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5160,7 +5509,7 @@
         <v>79</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -5171,7 +5520,7 @@
         <v>80</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -5182,7 +5531,7 @@
         <v>81</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5193,7 +5542,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="85" x14ac:dyDescent="0.2">
@@ -5204,7 +5553,7 @@
         <v>83</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5215,7 +5564,7 @@
         <v>84</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5226,7 +5575,7 @@
         <v>85</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5237,7 +5586,7 @@
         <v>86</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5248,7 +5597,7 @@
         <v>87</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5259,7 +5608,7 @@
         <v>88</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -5270,7 +5619,7 @@
         <v>89</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Team 7 project report
</commit_message>
<xml_diff>
--- a/Team7ProjectReport.xlsx
+++ b/Team7ProjectReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/Week4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/week9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F705A11-5EBF-244C-A2F8-D0F9A0FF59AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F72EF70-5821-A645-BBE9-831E42BDE9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" activeTab="5" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="201">
   <si>
     <t>First</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -646,6 +646,15 @@
   </si>
   <si>
     <t>Child should be born before the death of the mother and before 9 months after the death of the father</t>
+  </si>
+  <si>
+    <t>Avoid:</t>
+  </si>
+  <si>
+    <t>leaving discussions for the last minutes</t>
+  </si>
+  <si>
+    <t>peer-review of the User Story developed by each team member and providing feedbacks to improve the script.</t>
   </si>
 </sst>
 </file>
@@ -1212,9 +1221,19 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.2692038495188109E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
+          <c:w val="0.90286351706036749"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
-        <c:grouping val="standard"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1245,10 +1264,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Burndown!$A$3:$A$7</c:f>
+              <c:f>Burndown!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>45079</c:v>
                 </c:pt>
@@ -1262,17 +1281,20 @@
                   <c:v>45120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45133</c:v>
+                  <c:v>45134</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$B$3:$B$7</c:f>
+              <c:f>Burndown!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
@@ -1288,13 +1310,16 @@
                 <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D05B-2948-AB38-DD69DF259275}"/>
+              <c16:uniqueId val="{00000000-3F7C-1E48-A2A2-93F30B4412D1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1308,11 +1333,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68874927"/>
-        <c:axId val="68876575"/>
+        <c:axId val="98989391"/>
+        <c:axId val="98987503"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68874927"/>
+        <c:axId val="98989391"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1355,14 +1380,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68876575"/>
+        <c:crossAx val="98987503"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68876575"/>
+        <c:axId val="98987503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1438,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68874927"/>
+        <c:crossAx val="98989391"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1426,7 +1451,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3166,22 +3191,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29AFAAB0-08BD-70CB-76CC-1020FC0A9B03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E78ABCB1-FE05-9BD9-0C49-15AB33FA64D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3502,7 +3527,7 @@
   <dimension ref="A3:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3643,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6468BA2-C19E-AA4E-A2B7-75FD15389C5C}">
   <dimension ref="A3:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3956,7 +3981,7 @@
         <v>187</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3973,7 +3998,7 @@
         <v>187</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3990,7 +4015,7 @@
         <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -4007,7 +4032,7 @@
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -4024,7 +4049,7 @@
         <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -4041,7 +4066,7 @@
         <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -4058,7 +4083,7 @@
         <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -4075,7 +4100,7 @@
         <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4088,6 +4113,9 @@
       <c r="C28" t="s">
         <v>82</v>
       </c>
+      <c r="E28" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -4099,6 +4127,9 @@
       <c r="C29" t="s">
         <v>83</v>
       </c>
+      <c r="E29" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -4110,6 +4141,9 @@
       <c r="C30" t="s">
         <v>84</v>
       </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -4121,6 +4155,9 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -4132,8 +4169,11 @@
       <c r="C32" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -4143,8 +4183,11 @@
       <c r="C33" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -4154,8 +4197,11 @@
       <c r="C34" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -4164,6 +4210,9 @@
       </c>
       <c r="C35" t="s">
         <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4176,8 +4225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F2ECB25-720D-8D47-86EC-308937FE2D00}">
   <dimension ref="A3:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4278,7 +4327,9 @@
         <v>0</v>
       </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -4299,7 +4350,9 @@
       <c r="F21" s="11">
         <v>165</v>
       </c>
-      <c r="G21" s="7"/>
+      <c r="G21">
+        <v>160</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -4320,7 +4373,9 @@
       <c r="F22" s="11">
         <v>145</v>
       </c>
-      <c r="G22" s="7"/>
+      <c r="G22">
+        <v>120</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -4336,12 +4391,14 @@
         <v>8</v>
       </c>
       <c r="E23" s="11">
-        <v>0</v>
+        <v>820</v>
       </c>
       <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>220</v>
+      </c>
+      <c r="G23">
+        <v>182</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
@@ -4376,10 +4433,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C644DD-ABBB-504B-B47B-7D78685436AC}">
-  <dimension ref="A2:F7"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F4" sqref="F4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4463,16 +4520,39 @@
       <c r="A6" s="10">
         <v>45120</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>16</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>820</v>
+      </c>
+      <c r="E6" s="12">
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
-        <v>45133</v>
+        <v>45134</v>
       </c>
       <c r="B7">
         <v>8</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>45148</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4486,7 +4566,7 @@
   <dimension ref="A2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4767,8 +4847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E5BDE68-3A09-9D41-98E9-14B644F01EC8}">
   <dimension ref="A3:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5073,15 +5153,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4605CCB-00E7-694D-83D4-7E84E084E5F6}">
-  <dimension ref="A3:I11"/>
+  <dimension ref="A3:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.2">
@@ -5124,7 +5206,22 @@
         <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E4" s="17">
+        <v>30</v>
+      </c>
+      <c r="F4" s="5">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17">
+        <v>40</v>
+      </c>
+      <c r="H4" s="5">
+        <v>20</v>
+      </c>
+      <c r="I4" s="18">
+        <v>45134</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -5138,7 +5235,22 @@
         <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E5" s="17">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5">
+        <v>30</v>
+      </c>
+      <c r="G5" s="17">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>20</v>
+      </c>
+      <c r="I5" s="18">
+        <v>45134</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -5152,7 +5264,22 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E6" s="17">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5">
+        <v>25</v>
+      </c>
+      <c r="G6" s="17">
+        <v>38</v>
+      </c>
+      <c r="H6" s="17">
+        <v>15</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45133</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -5166,7 +5293,22 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E7" s="17">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5">
+        <v>25</v>
+      </c>
+      <c r="G7" s="17">
+        <v>45</v>
+      </c>
+      <c r="H7" s="17">
+        <v>20</v>
+      </c>
+      <c r="I7" s="18">
+        <v>45133</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -5180,7 +5322,22 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E8" s="17">
+        <v>20</v>
+      </c>
+      <c r="F8" s="5">
+        <v>20</v>
+      </c>
+      <c r="G8" s="17">
+        <v>29</v>
+      </c>
+      <c r="H8" s="17">
+        <v>20</v>
+      </c>
+      <c r="I8" s="18">
+        <v>45133</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -5194,7 +5351,22 @@
         <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E9" s="17">
+        <v>25</v>
+      </c>
+      <c r="F9" s="5">
+        <v>20</v>
+      </c>
+      <c r="G9" s="17">
+        <v>17</v>
+      </c>
+      <c r="H9" s="17">
+        <v>15</v>
+      </c>
+      <c r="I9" s="18">
+        <v>45133</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -5208,7 +5380,22 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E10" s="17">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5">
+        <v>25</v>
+      </c>
+      <c r="G10" s="17">
+        <v>20</v>
+      </c>
+      <c r="H10" s="17">
+        <v>15</v>
+      </c>
+      <c r="I10" s="18">
+        <v>45132</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -5222,7 +5409,38 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="E11" s="17">
+        <v>15</v>
+      </c>
+      <c r="F11" s="17">
+        <v>25</v>
+      </c>
+      <c r="G11" s="17">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17">
+        <v>20</v>
+      </c>
+      <c r="I11" s="18">
+        <v>45132</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="J17" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J19" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="K19" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -5233,14 +5451,159 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B21356-0FF2-604A-A31D-9402F229508C}">
-  <dimension ref="A1"/>
+  <dimension ref="A5:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5249,8 +5612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E792817E-5E9F-5543-BCFF-41F35057F086}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5625,5 +5988,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added project report for sprint 4
</commit_message>
<xml_diff>
--- a/Team7ProjectReport.xlsx
+++ b/Team7ProjectReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/week9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/week11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F72EF70-5821-A645-BBE9-831E42BDE9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5040A8FE-AFC1-1146-9424-EAD18910F1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="7" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="203">
   <si>
     <t>First</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -655,6 +655,12 @@
   </si>
   <si>
     <t>peer-review of the User Story developed by each team member and providing feedbacks to improve the script.</t>
+  </si>
+  <si>
+    <t>following same way of communication, equal involvemen and contribution, peer-review and feedbacks.</t>
+  </si>
+  <si>
+    <t>implementing the Sprints at last day.</t>
   </si>
 </sst>
 </file>
@@ -3668,8 +3674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6468BA2-C19E-AA4E-A2B7-75FD15389C5C}">
   <dimension ref="A3:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E35"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4114,7 +4120,7 @@
         <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4128,7 +4134,7 @@
         <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -4142,7 +4148,7 @@
         <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -4156,7 +4162,7 @@
         <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4170,7 +4176,7 @@
         <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -4184,7 +4190,7 @@
         <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -4198,7 +4204,7 @@
         <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -4212,7 +4218,7 @@
         <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4226,7 +4232,7 @@
   <dimension ref="A3:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4414,12 +4420,14 @@
         <v>8</v>
       </c>
       <c r="E24" s="11">
-        <v>0</v>
+        <v>1024</v>
       </c>
       <c r="F24" s="11">
-        <v>0</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>440</v>
+      </c>
+      <c r="G24">
+        <v>320</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
@@ -4436,7 +4444,7 @@
   <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4540,18 +4548,30 @@
       <c r="A7" s="10">
         <v>45134</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="12">
         <v>8</v>
       </c>
       <c r="C7">
         <v>8</v>
+      </c>
+      <c r="D7">
+        <v>1024</v>
+      </c>
+      <c r="E7" s="12">
+        <v>440</v>
+      </c>
+      <c r="F7">
+        <v>320</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>45148</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>0</v>
       </c>
     </row>
@@ -4566,7 +4586,7 @@
   <dimension ref="A2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H7" sqref="H7:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4848,7 +4868,7 @@
   <dimension ref="A3:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="G4" sqref="G4:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5156,7 +5176,7 @@
   <dimension ref="A3:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J17" sqref="J17:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5451,18 +5471,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B21356-0FF2-604A-A31D-9402F229508C}">
-  <dimension ref="A5:I13"/>
+  <dimension ref="A5:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="11" max="11" width="38.83203125" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>108</v>
       </c>
@@ -5504,6 +5525,21 @@
       <c r="D6" t="s">
         <v>65</v>
       </c>
+      <c r="E6" s="17">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6" s="17">
+        <v>40</v>
+      </c>
+      <c r="H6" s="5">
+        <v>20</v>
+      </c>
+      <c r="I6" s="18">
+        <v>45147</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5518,6 +5554,21 @@
       <c r="D7" t="s">
         <v>65</v>
       </c>
+      <c r="E7" s="17">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="G7" s="17">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5">
+        <v>15</v>
+      </c>
+      <c r="I7" s="18">
+        <v>45147</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5532,6 +5583,21 @@
       <c r="D8" t="s">
         <v>65</v>
       </c>
+      <c r="E8" s="17">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8" s="17">
+        <v>38</v>
+      </c>
+      <c r="H8" s="17">
+        <v>15</v>
+      </c>
+      <c r="I8" s="18">
+        <v>45146</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5546,6 +5612,21 @@
       <c r="D9" t="s">
         <v>65</v>
       </c>
+      <c r="E9" s="17">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9" s="17">
+        <v>45</v>
+      </c>
+      <c r="H9" s="17">
+        <v>10</v>
+      </c>
+      <c r="I9" s="18">
+        <v>45146</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5560,6 +5641,21 @@
       <c r="D10" t="s">
         <v>65</v>
       </c>
+      <c r="E10" s="17">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" s="17">
+        <v>29</v>
+      </c>
+      <c r="H10" s="17">
+        <v>10</v>
+      </c>
+      <c r="I10" s="18">
+        <v>45145</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5574,6 +5670,21 @@
       <c r="D11" t="s">
         <v>65</v>
       </c>
+      <c r="E11" s="17">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11" s="17">
+        <v>17</v>
+      </c>
+      <c r="H11" s="17">
+        <v>15</v>
+      </c>
+      <c r="I11" s="18">
+        <v>45145</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5588,6 +5699,21 @@
       <c r="D12" t="s">
         <v>65</v>
       </c>
+      <c r="E12" s="17">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>25</v>
+      </c>
+      <c r="G12" s="17">
+        <v>20</v>
+      </c>
+      <c r="H12" s="17">
+        <v>20</v>
+      </c>
+      <c r="I12" s="18">
+        <v>45146</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -5601,6 +5727,42 @@
       </c>
       <c r="D13" t="s">
         <v>65</v>
+      </c>
+      <c r="E13" s="17">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>15</v>
+      </c>
+      <c r="G13" s="17">
+        <v>35</v>
+      </c>
+      <c r="H13" s="17">
+        <v>10</v>
+      </c>
+      <c r="I13" s="18">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="J18" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="J20" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -5612,8 +5774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E792817E-5E9F-5543-BCFF-41F35057F086}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated Test report For sprint 4
</commit_message>
<xml_diff>
--- a/Team7ProjectReport.xlsx
+++ b/Team7ProjectReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priyankakoul/Documents/Stevens/Stevens_Study/Core_courses/SSW-555_Agile Methods for SW Dev/Assignments/week11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5040A8FE-AFC1-1146-9424-EAD18910F1FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576849A1-4B89-264E-852E-6FE2A914F52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="7" xr2:uid="{4A9CD5A7-A6D9-4244-BF95-5B9BEAE451A2}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="203">
   <si>
     <t>First</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -3675,7 +3675,7 @@
   <dimension ref="A3:E35"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E35"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4119,6 +4119,9 @@
       <c r="C28" t="s">
         <v>82</v>
       </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
       <c r="E28" t="s">
         <v>193</v>
       </c>
@@ -4133,6 +4136,9 @@
       <c r="C29" t="s">
         <v>83</v>
       </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
       <c r="E29" t="s">
         <v>193</v>
       </c>
@@ -4147,6 +4153,9 @@
       <c r="C30" t="s">
         <v>84</v>
       </c>
+      <c r="D30" t="s">
+        <v>187</v>
+      </c>
       <c r="E30" t="s">
         <v>193</v>
       </c>
@@ -4161,6 +4170,9 @@
       <c r="C31" t="s">
         <v>85</v>
       </c>
+      <c r="D31" t="s">
+        <v>187</v>
+      </c>
       <c r="E31" t="s">
         <v>193</v>
       </c>
@@ -4175,6 +4187,9 @@
       <c r="C32" t="s">
         <v>86</v>
       </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
       <c r="E32" t="s">
         <v>193</v>
       </c>
@@ -4189,6 +4204,9 @@
       <c r="C33" t="s">
         <v>87</v>
       </c>
+      <c r="D33" t="s">
+        <v>34</v>
+      </c>
       <c r="E33" t="s">
         <v>193</v>
       </c>
@@ -4203,6 +4221,9 @@
       <c r="C34" t="s">
         <v>88</v>
       </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
       <c r="E34" t="s">
         <v>193</v>
       </c>
@@ -4216,6 +4237,9 @@
       </c>
       <c r="C35" t="s">
         <v>89</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
       </c>
       <c r="E35" t="s">
         <v>193</v>
@@ -5474,7 +5498,7 @@
   <dimension ref="A5:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5520,7 +5544,7 @@
         <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>65</v>
@@ -5549,7 +5573,7 @@
         <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>65</v>
@@ -5578,7 +5602,7 @@
         <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>187</v>
       </c>
       <c r="D8" t="s">
         <v>65</v>
@@ -5607,7 +5631,7 @@
         <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
         <v>65</v>

</xml_diff>